<commit_message>
<fix> description, authors and editorials in book required fixed
</commit_message>
<xml_diff>
--- a/Ejemplo formato libros de biblioteca.xlsx
+++ b/Ejemplo formato libros de biblioteca.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnologia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tecnologia\Desktop\gabo\iujo-biblioteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A6F0DD-4351-47C6-BCB3-71655FEBB389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3505E6-83A7-4222-B6DB-E29339007207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Título</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Relata el ficticio nacimiento de un horror cósmico cuya presencia resuena en las mentes y cuerpos de todas las personas y seres</t>
   </si>
   <si>
-    <t>Trata de las ocurrencias, aventuras y vivencias de un caballero medieval delirantemente obsesionado con las costumbres caballerescas de la edad media</t>
-  </si>
-  <si>
     <t>Berserk Vol. 1</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>Hakusensha</t>
-  </si>
-  <si>
-    <t>Cuenta la historia de un misterioso y oscuro espadachín que lucha contra monstruos que se alzan en su contra por alguna razón</t>
   </si>
   <si>
     <t>Estante</t>
@@ -518,7 +512,7 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -539,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -548,13 +542,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
@@ -568,7 +562,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -580,7 +574,7 @@
         <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
@@ -594,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
@@ -606,7 +600,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -620,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -632,101 +626,95 @@
         <v>225</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="2">
         <v>220</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>